<commit_message>
schematic for low cost rf front end
narrowband version for rf shield with max2832 receiver can be founf at
HW/frontend/RFshield/max2832version
</commit_message>
<xml_diff>
--- a/HW/frontend/RFshield/bomrfshieldfull.xlsx
+++ b/HW/frontend/RFshield/bomrfshieldfull.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="258">
   <si>
     <t>R18</t>
   </si>
@@ -655,12 +655,6 @@
   </si>
   <si>
     <t>c44</t>
-  </si>
-  <si>
-    <t>p37</t>
-  </si>
-  <si>
-    <t>p33</t>
   </si>
   <si>
     <t>l1</t>
@@ -828,12 +822,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -849,12 +849,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1136,10 +1138,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J120"/>
+  <dimension ref="A1:J117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1153,7 +1155,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -1188,7 +1190,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -1311,7 +1313,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C6" t="s">
         <v>143</v>
@@ -1371,7 +1373,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C8" t="s">
         <v>143</v>
@@ -1401,7 +1403,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C9" t="s">
         <v>143</v>
@@ -1611,7 +1613,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C16" t="s">
         <v>28</v>
@@ -1641,7 +1643,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
@@ -1671,7 +1673,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
@@ -1701,7 +1703,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C19" t="s">
         <v>38</v>
@@ -1731,7 +1733,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C20" t="s">
         <v>38</v>
@@ -1791,7 +1793,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C22" t="s">
         <v>38</v>
@@ -2211,7 +2213,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C36" t="s">
         <v>38</v>
@@ -2721,7 +2723,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C53" t="s">
         <v>28</v>
@@ -3159,7 +3161,7 @@
         <v>0.1</v>
       </c>
       <c r="H67">
-        <f t="shared" ref="H67:H119" si="1">G67*F67</f>
+        <f t="shared" ref="H67:H116" si="1">G67*F67</f>
         <v>0.1</v>
       </c>
       <c r="I67" t="s">
@@ -3321,7 +3323,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C73" t="s">
         <v>46</v>
@@ -3351,70 +3353,90 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>210</v>
+        <v>71</v>
+      </c>
+      <c r="C74" t="s">
+        <v>70</v>
       </c>
       <c r="F74">
         <v>1</v>
       </c>
+      <c r="G74">
+        <v>18.64</v>
+      </c>
       <c r="H74">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>18.64</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
-      <c r="B75" t="s">
-        <v>211</v>
-      </c>
-      <c r="F75">
-        <v>1</v>
-      </c>
-      <c r="H75">
+      <c r="B75" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3">
+        <v>1</v>
+      </c>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="I75" s="4"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
-      <c r="B76" t="s">
-        <v>71</v>
-      </c>
-      <c r="C76" t="s">
-        <v>70</v>
-      </c>
-      <c r="F76">
-        <v>1</v>
-      </c>
-      <c r="G76">
-        <v>18.64</v>
-      </c>
-      <c r="H76">
-        <f t="shared" si="1"/>
-        <v>18.64</v>
-      </c>
-      <c r="I76" s="2" t="s">
-        <v>69</v>
-      </c>
+      <c r="B76" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3">
+        <v>1</v>
+      </c>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I76" s="4"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="F77">
-        <v>1</v>
-      </c>
-      <c r="H77">
+      <c r="C77" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3">
+        <v>1</v>
+      </c>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I77" s="2"/>
+      <c r="I77" s="3"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
@@ -3423,43 +3445,87 @@
       <c r="B78" t="s">
         <v>213</v>
       </c>
+      <c r="C78" t="s">
+        <v>28</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78" t="s">
+        <v>29</v>
+      </c>
       <c r="F78">
         <v>1</v>
       </c>
+      <c r="G78">
+        <v>0.1</v>
+      </c>
       <c r="H78">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I78" s="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I78" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>214</v>
+        <v>246</v>
       </c>
       <c r="C79" t="s">
-        <v>72</v>
+        <v>28</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79" t="s">
+        <v>29</v>
       </c>
       <c r="F79">
         <v>1</v>
       </c>
+      <c r="G79">
+        <v>0.1</v>
+      </c>
       <c r="H79">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
+      </c>
+      <c r="I79" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
+      <c r="B80" t="s">
+        <v>249</v>
+      </c>
+      <c r="C80" t="s">
+        <v>28</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80" t="s">
+        <v>29</v>
+      </c>
       <c r="F80">
         <v>1</v>
       </c>
+      <c r="G80">
+        <v>0.1</v>
+      </c>
       <c r="H80">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
+      </c>
+      <c r="I80" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -3467,7 +3533,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>215</v>
+        <v>250</v>
       </c>
       <c r="C81" t="s">
         <v>28</v>
@@ -3497,7 +3563,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C82" t="s">
         <v>28</v>
@@ -3527,7 +3593,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C83" t="s">
         <v>28</v>
@@ -3557,7 +3623,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C84" t="s">
         <v>28</v>
@@ -3587,7 +3653,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C85" t="s">
         <v>28</v>
@@ -3617,7 +3683,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C86" t="s">
         <v>28</v>
@@ -3647,7 +3713,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C87" t="s">
         <v>28</v>
@@ -3677,29 +3743,29 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>256</v>
+        <v>73</v>
       </c>
       <c r="C88" t="s">
-        <v>28</v>
-      </c>
-      <c r="D88">
-        <v>0</v>
+        <v>74</v>
+      </c>
+      <c r="D88" t="s">
+        <v>75</v>
       </c>
       <c r="E88" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="F88">
         <v>1</v>
       </c>
       <c r="G88">
-        <v>0.1</v>
+        <v>1.08</v>
       </c>
       <c r="H88">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>1.08</v>
       </c>
       <c r="I88" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -3707,29 +3773,29 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>257</v>
+        <v>79</v>
       </c>
       <c r="C89" t="s">
-        <v>28</v>
-      </c>
-      <c r="D89">
-        <v>0</v>
+        <v>80</v>
+      </c>
+      <c r="D89" t="s">
+        <v>81</v>
       </c>
       <c r="E89" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="F89">
         <v>1</v>
       </c>
       <c r="G89">
-        <v>0.1</v>
+        <v>2.1019999999999999</v>
       </c>
       <c r="H89">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>2.1019999999999999</v>
       </c>
       <c r="I89" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -3737,29 +3803,29 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>258</v>
+        <v>216</v>
       </c>
       <c r="C90" t="s">
-        <v>28</v>
-      </c>
-      <c r="D90">
-        <v>0</v>
+        <v>83</v>
+      </c>
+      <c r="D90" t="s">
+        <v>84</v>
       </c>
       <c r="E90" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="F90">
         <v>1</v>
       </c>
       <c r="G90">
-        <v>0.1</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="H90">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="I90" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -3767,29 +3833,29 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>73</v>
+        <v>217</v>
       </c>
       <c r="C91" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="D91" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E91" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="F91">
         <v>1</v>
       </c>
       <c r="G91">
-        <v>1.08</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="H91">
         <f t="shared" si="1"/>
-        <v>1.08</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="I91" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -3797,29 +3863,29 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>79</v>
+        <v>218</v>
       </c>
       <c r="C92" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="D92" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E92" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="F92">
         <v>1</v>
       </c>
       <c r="G92">
-        <v>2.1019999999999999</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="H92">
         <f t="shared" si="1"/>
-        <v>2.1019999999999999</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="I92" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -3827,29 +3893,29 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C93" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="D93" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E93" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F93">
         <v>1</v>
       </c>
       <c r="G93">
-        <v>0.57999999999999996</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="H93">
         <f t="shared" si="1"/>
-        <v>0.57999999999999996</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="I93" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -3857,29 +3923,29 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C94" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="D94" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="E94" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="F94">
         <v>1</v>
       </c>
       <c r="G94">
-        <v>0.57999999999999996</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="H94">
         <f t="shared" si="1"/>
-        <v>0.57999999999999996</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="I94" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -3887,29 +3953,29 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C95" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="D95" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E95" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="F95">
         <v>1</v>
       </c>
       <c r="G95">
-        <v>2.1000000000000001E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="H95">
         <f t="shared" si="1"/>
-        <v>2.1000000000000001E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="I95" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -3917,29 +3983,29 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C96" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="D96" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E96" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="F96">
         <v>1</v>
       </c>
       <c r="G96">
-        <v>2.1000000000000001E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="H96">
         <f t="shared" si="1"/>
-        <v>2.1000000000000001E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="I96" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -3947,29 +4013,26 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>222</v>
+        <v>93</v>
       </c>
       <c r="C97" t="s">
-        <v>90</v>
-      </c>
-      <c r="D97" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E97" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F97">
         <v>1</v>
       </c>
       <c r="G97">
-        <v>8.4000000000000005E-2</v>
+        <v>9.23</v>
       </c>
       <c r="H97">
         <f t="shared" si="1"/>
-        <v>8.4000000000000005E-2</v>
+        <v>9.23</v>
       </c>
       <c r="I97" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -3977,29 +4040,29 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>223</v>
+        <v>99</v>
       </c>
       <c r="C98" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D98" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="E98" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="F98">
         <v>1</v>
       </c>
       <c r="G98">
-        <v>8.4000000000000005E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="H98">
         <f t="shared" si="1"/>
-        <v>8.4000000000000005E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="I98" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -4010,26 +4073,26 @@
         <v>224</v>
       </c>
       <c r="C99" t="s">
-        <v>90</v>
-      </c>
-      <c r="D99" t="s">
-        <v>91</v>
+        <v>28</v>
+      </c>
+      <c r="D99">
+        <v>475</v>
       </c>
       <c r="E99" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="F99">
         <v>1</v>
       </c>
       <c r="G99">
-        <v>8.4000000000000005E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="H99">
         <f t="shared" si="1"/>
-        <v>8.4000000000000005E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="I99" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -4037,26 +4100,29 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>93</v>
+        <v>225</v>
       </c>
       <c r="C100" t="s">
-        <v>92</v>
+        <v>28</v>
+      </c>
+      <c r="D100">
+        <v>475</v>
       </c>
       <c r="E100" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="F100">
         <v>1</v>
       </c>
       <c r="G100">
-        <v>9.23</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="H100">
         <f t="shared" si="1"/>
-        <v>9.23</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="I100" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -4064,29 +4130,29 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>99</v>
+        <v>226</v>
       </c>
       <c r="C101" t="s">
-        <v>100</v>
+        <v>38</v>
       </c>
       <c r="D101" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="E101" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="F101">
         <v>1</v>
       </c>
       <c r="G101">
-        <v>4.5999999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="H101">
         <f t="shared" si="1"/>
-        <v>4.5999999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="I101" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -4094,29 +4160,29 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C102" t="s">
-        <v>28</v>
-      </c>
-      <c r="D102">
-        <v>475</v>
+        <v>110</v>
+      </c>
+      <c r="D102" t="s">
+        <v>108</v>
       </c>
       <c r="E102" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="F102">
         <v>1</v>
       </c>
       <c r="G102">
-        <v>1.2999999999999999E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="H102">
         <f t="shared" si="1"/>
-        <v>1.2999999999999999E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="I102" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -4124,16 +4190,16 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>227</v>
+        <v>112</v>
       </c>
       <c r="C103" t="s">
         <v>28</v>
       </c>
       <c r="D103">
-        <v>475</v>
+        <v>39</v>
       </c>
       <c r="E103" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="F103">
         <v>1</v>
@@ -4145,8 +4211,8 @@
         <f t="shared" si="1"/>
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="I103" t="s">
-        <v>104</v>
+      <c r="I103" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -4154,29 +4220,29 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="C104" t="s">
-        <v>38</v>
-      </c>
-      <c r="D104" t="s">
-        <v>105</v>
+        <v>28</v>
+      </c>
+      <c r="D104">
+        <v>39</v>
       </c>
       <c r="E104" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="F104">
         <v>1</v>
       </c>
       <c r="G104">
-        <v>2.3E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="H104">
         <f t="shared" si="1"/>
-        <v>2.3E-2</v>
-      </c>
-      <c r="I104" t="s">
-        <v>107</v>
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="I104" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
@@ -4184,29 +4250,29 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="C105" t="s">
-        <v>110</v>
-      </c>
-      <c r="D105" t="s">
-        <v>108</v>
+        <v>28</v>
+      </c>
+      <c r="D105">
+        <v>39</v>
       </c>
       <c r="E105" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F105">
         <v>1</v>
       </c>
       <c r="G105">
-        <v>2.8000000000000001E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="H105">
         <f t="shared" si="1"/>
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="I105" t="s">
-        <v>111</v>
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="I105" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
@@ -4214,7 +4280,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>112</v>
+        <v>239</v>
       </c>
       <c r="C106" t="s">
         <v>28</v>
@@ -4244,29 +4310,26 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>235</v>
+        <v>115</v>
       </c>
       <c r="C107" t="s">
-        <v>28</v>
-      </c>
-      <c r="D107">
-        <v>39</v>
+        <v>116</v>
       </c>
       <c r="E107" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F107">
         <v>1</v>
       </c>
       <c r="G107">
-        <v>1.2999999999999999E-2</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="H107">
         <f t="shared" si="1"/>
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="I107" s="2" t="s">
-        <v>114</v>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="I107" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -4274,29 +4337,26 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C108" t="s">
-        <v>28</v>
-      </c>
-      <c r="D108">
-        <v>39</v>
+        <v>120</v>
       </c>
       <c r="E108" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="F108">
         <v>1</v>
       </c>
       <c r="G108">
-        <v>1.2999999999999999E-2</v>
+        <v>0.38400000000000001</v>
       </c>
       <c r="H108">
         <f t="shared" si="1"/>
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="I108" s="2" t="s">
-        <v>114</v>
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="I108" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
@@ -4304,29 +4364,26 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C109" t="s">
-        <v>28</v>
-      </c>
-      <c r="D109">
-        <v>39</v>
+        <v>120</v>
       </c>
       <c r="E109" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="F109">
         <v>1</v>
       </c>
       <c r="G109">
-        <v>1.2999999999999999E-2</v>
+        <v>0.38400000000000001</v>
       </c>
       <c r="H109">
         <f t="shared" si="1"/>
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="I109" s="2" t="s">
-        <v>114</v>
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="I109" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -4334,26 +4391,29 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="C110" t="s">
-        <v>116</v>
+        <v>124</v>
+      </c>
+      <c r="D110" t="s">
+        <v>240</v>
       </c>
       <c r="E110" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="F110">
         <v>1</v>
       </c>
       <c r="G110">
-        <v>0.28999999999999998</v>
+        <v>1.6E-2</v>
       </c>
       <c r="H110">
         <f t="shared" si="1"/>
-        <v>0.28999999999999998</v>
+        <v>1.6E-2</v>
       </c>
       <c r="I110" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
@@ -4361,26 +4421,29 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>237</v>
+        <v>127</v>
       </c>
       <c r="C111" t="s">
-        <v>120</v>
+        <v>128</v>
+      </c>
+      <c r="D111" t="s">
+        <v>241</v>
       </c>
       <c r="E111" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="F111">
         <v>1</v>
       </c>
       <c r="G111">
-        <v>0.38400000000000001</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="H111">
         <f t="shared" si="1"/>
-        <v>0.38400000000000001</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="I111" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -4388,218 +4451,141 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>238</v>
+        <v>131</v>
       </c>
       <c r="C112" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E112" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="F112">
         <v>1</v>
       </c>
       <c r="G112">
-        <v>0.38400000000000001</v>
+        <v>2.93</v>
       </c>
       <c r="H112">
         <f t="shared" si="1"/>
-        <v>0.38400000000000001</v>
+        <v>2.93</v>
       </c>
       <c r="I112" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="C113" t="s">
-        <v>124</v>
-      </c>
-      <c r="D113" t="s">
-        <v>242</v>
+        <v>135</v>
       </c>
       <c r="E113" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="F113">
         <v>1</v>
       </c>
       <c r="G113">
-        <v>1.6E-2</v>
+        <v>3.8</v>
       </c>
       <c r="H113">
         <f t="shared" si="1"/>
-        <v>1.6E-2</v>
+        <v>3.8</v>
       </c>
       <c r="I113" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C114" t="s">
-        <v>128</v>
-      </c>
-      <c r="D114" t="s">
-        <v>243</v>
+        <v>136</v>
       </c>
       <c r="E114" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="F114">
         <v>1</v>
       </c>
       <c r="G114">
-        <v>1.2999999999999999E-2</v>
+        <v>2.9</v>
       </c>
       <c r="H114">
         <f t="shared" si="1"/>
-        <v>1.2999999999999999E-2</v>
+        <v>2.9</v>
       </c>
       <c r="I114" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
-      <c r="B115" t="s">
-        <v>131</v>
-      </c>
-      <c r="C115" t="s">
-        <v>130</v>
-      </c>
-      <c r="E115" t="s">
-        <v>138</v>
-      </c>
-      <c r="F115">
-        <v>1</v>
-      </c>
-      <c r="G115">
-        <v>2.93</v>
-      </c>
-      <c r="H115">
-        <f t="shared" si="1"/>
-        <v>2.93</v>
-      </c>
-      <c r="I115" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B115" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D115" s="3"/>
+      <c r="E115" s="3"/>
+      <c r="F115" s="3">
+        <v>1</v>
+      </c>
+      <c r="G115" s="3"/>
+      <c r="H115" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I115" s="3"/>
+      <c r="J115" s="3"/>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
-      <c r="B116" t="s">
-        <v>132</v>
-      </c>
-      <c r="C116" t="s">
-        <v>135</v>
-      </c>
-      <c r="E116" t="s">
-        <v>134</v>
-      </c>
-      <c r="F116">
-        <v>1</v>
-      </c>
-      <c r="G116">
-        <v>3.8</v>
-      </c>
-      <c r="H116">
-        <f t="shared" si="1"/>
-        <v>3.8</v>
-      </c>
-      <c r="I116" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A117">
-        <v>116</v>
-      </c>
-      <c r="B117" t="s">
-        <v>133</v>
-      </c>
-      <c r="C117" t="s">
-        <v>136</v>
-      </c>
-      <c r="E117" t="s">
-        <v>139</v>
-      </c>
-      <c r="F117">
-        <v>1</v>
-      </c>
-      <c r="G117">
-        <v>2.9</v>
-      </c>
+      <c r="B116" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D116" s="3"/>
+      <c r="E116" s="3"/>
+      <c r="F116" s="3">
+        <v>1</v>
+      </c>
+      <c r="G116" s="3"/>
+      <c r="H116" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I116" s="3"/>
+      <c r="J116" s="3"/>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H117">
-        <f t="shared" si="1"/>
-        <v>2.9</v>
-      </c>
-      <c r="I117" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A118">
-        <v>117</v>
-      </c>
-      <c r="B118" t="s">
-        <v>245</v>
-      </c>
-      <c r="C118" t="s">
-        <v>247</v>
-      </c>
-      <c r="F118">
-        <v>1</v>
-      </c>
-      <c r="H118">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A119">
-        <v>118</v>
-      </c>
-      <c r="B119" t="s">
-        <v>246</v>
-      </c>
-      <c r="C119" t="s">
-        <v>247</v>
-      </c>
-      <c r="F119">
-        <v>1</v>
-      </c>
-      <c r="H119">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H120">
-        <f>SUM(H2:H119)</f>
+        <f>SUM(H2:H116)</f>
         <v>61.157000000000011</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I109" r:id="rId1"/>
-    <hyperlink ref="I76" r:id="rId2"/>
-    <hyperlink ref="I106" r:id="rId3"/>
-    <hyperlink ref="I108" r:id="rId4"/>
-    <hyperlink ref="I107" r:id="rId5"/>
+    <hyperlink ref="I106" r:id="rId1"/>
+    <hyperlink ref="I74" r:id="rId2"/>
+    <hyperlink ref="I103" r:id="rId3"/>
+    <hyperlink ref="I105" r:id="rId4"/>
+    <hyperlink ref="I104" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
smd discrete components switched to 0402 package
</commit_message>
<xml_diff>
--- a/HW/frontend/RFshield/bomrfshieldfull.xlsx
+++ b/HW/frontend/RFshield/bomrfshieldfull.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -300,9 +299,6 @@
     <t>CAP CER 0.33UF 10V X5R 0402</t>
   </si>
   <si>
-    <t>0,33 pf</t>
-  </si>
-  <si>
     <t>MAX5864</t>
   </si>
   <si>
@@ -799,6 +795,9 @@
   </si>
   <si>
     <t>numero</t>
+  </si>
+  <si>
+    <t>0,33 uf</t>
   </si>
 </sst>
 </file>
@@ -1138,10 +1137,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J117"/>
+  <dimension ref="A1:J118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E109" sqref="E109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,7 +1154,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -1190,7 +1189,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -1238,7 +1237,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H66" si="0">G3*F3</f>
+        <f t="shared" ref="H3:H67" si="0">G3*F3</f>
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="I3" t="s">
@@ -1313,10 +1312,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D6">
         <v>50</v>
@@ -1343,10 +1342,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" t="s">
         <v>142</v>
-      </c>
-      <c r="C7" t="s">
-        <v>143</v>
       </c>
       <c r="D7">
         <v>50</v>
@@ -1373,10 +1372,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D8">
         <v>50</v>
@@ -1403,10 +1402,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D9">
         <v>50</v>
@@ -1463,7 +1462,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C11" t="s">
         <v>28</v>
@@ -1493,7 +1492,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C12" t="s">
         <v>28</v>
@@ -1553,7 +1552,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C14" t="s">
         <v>28</v>
@@ -1583,7 +1582,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C15" t="s">
         <v>28</v>
@@ -1613,7 +1612,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C16" t="s">
         <v>28</v>
@@ -1643,7 +1642,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
@@ -1673,7 +1672,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
@@ -1703,7 +1702,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C19" t="s">
         <v>38</v>
@@ -1733,7 +1732,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C20" t="s">
         <v>38</v>
@@ -1793,7 +1792,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C22" t="s">
         <v>38</v>
@@ -1853,7 +1852,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C24" t="s">
         <v>38</v>
@@ -1883,7 +1882,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C25" t="s">
         <v>38</v>
@@ -1913,7 +1912,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C26" t="s">
         <v>38</v>
@@ -1943,7 +1942,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C27" t="s">
         <v>38</v>
@@ -1973,7 +1972,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C28" t="s">
         <v>38</v>
@@ -2003,7 +2002,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C29" t="s">
         <v>38</v>
@@ -2033,7 +2032,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C30" t="s">
         <v>38</v>
@@ -2058,42 +2057,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>157</v>
-      </c>
-      <c r="C31" t="s">
-        <v>38</v>
-      </c>
-      <c r="D31" t="s">
-        <v>41</v>
-      </c>
-      <c r="E31" t="s">
-        <v>40</v>
-      </c>
-      <c r="F31">
-        <v>1</v>
-      </c>
-      <c r="G31">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="H31">
-        <f t="shared" si="0"/>
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="I31" t="s">
-        <v>42</v>
-      </c>
-    </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C32" t="s">
         <v>38</v>
@@ -2120,10 +2089,10 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C33" t="s">
         <v>38</v>
@@ -2150,10 +2119,10 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C34" t="s">
         <v>38</v>
@@ -2180,10 +2149,10 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C35" t="s">
         <v>38</v>
@@ -2210,10 +2179,10 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>228</v>
+        <v>160</v>
       </c>
       <c r="C36" t="s">
         <v>38</v>
@@ -2240,49 +2209,49 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>162</v>
+        <v>227</v>
       </c>
       <c r="C37" t="s">
         <v>38</v>
       </c>
       <c r="D37" t="s">
-        <v>163</v>
+        <v>41</v>
       </c>
       <c r="E37" t="s">
-        <v>164</v>
+        <v>40</v>
       </c>
       <c r="F37">
         <v>1</v>
       </c>
       <c r="G37">
-        <v>0.128</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="H37">
         <f t="shared" si="0"/>
-        <v>0.128</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="I37" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C38" t="s">
         <v>38</v>
       </c>
       <c r="D38" t="s">
+        <v>162</v>
+      </c>
+      <c r="E38" t="s">
         <v>163</v>
-      </c>
-      <c r="E38" t="s">
-        <v>164</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -2300,19 +2269,19 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C39" t="s">
         <v>38</v>
       </c>
       <c r="D39" t="s">
+        <v>162</v>
+      </c>
+      <c r="E39" t="s">
         <v>163</v>
-      </c>
-      <c r="E39" t="s">
-        <v>164</v>
       </c>
       <c r="F39">
         <v>1</v>
@@ -2330,19 +2299,19 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C40" t="s">
         <v>38</v>
       </c>
       <c r="D40" t="s">
+        <v>162</v>
+      </c>
+      <c r="E40" t="s">
         <v>163</v>
-      </c>
-      <c r="E40" t="s">
-        <v>164</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -2360,19 +2329,19 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C41" t="s">
         <v>38</v>
       </c>
       <c r="D41" t="s">
+        <v>162</v>
+      </c>
+      <c r="E41" t="s">
         <v>163</v>
-      </c>
-      <c r="E41" t="s">
-        <v>164</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -2390,19 +2359,19 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C42" t="s">
         <v>38</v>
       </c>
       <c r="D42" t="s">
+        <v>162</v>
+      </c>
+      <c r="E42" t="s">
         <v>163</v>
-      </c>
-      <c r="E42" t="s">
-        <v>164</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -2420,130 +2389,130 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>168</v>
       </c>
       <c r="C43" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D43" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="E43" t="s">
-        <v>47</v>
+        <v>163</v>
       </c>
       <c r="F43">
         <v>1</v>
       </c>
       <c r="G43">
-        <v>0.62</v>
+        <v>0.128</v>
       </c>
       <c r="H43">
         <f t="shared" si="0"/>
-        <v>0.62</v>
+        <v>0.128</v>
       </c>
       <c r="I43" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C44" t="s">
-        <v>49</v>
-      </c>
-      <c r="D44">
-        <v>220</v>
+        <v>46</v>
+      </c>
+      <c r="D44" t="s">
+        <v>45</v>
       </c>
       <c r="E44" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F44">
         <v>1</v>
       </c>
       <c r="G44">
-        <v>0.09</v>
+        <v>0.62</v>
       </c>
       <c r="H44">
         <f t="shared" si="0"/>
-        <v>0.09</v>
+        <v>0.62</v>
       </c>
       <c r="I44" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C45" t="s">
-        <v>46</v>
-      </c>
-      <c r="D45" t="s">
-        <v>53</v>
+        <v>49</v>
+      </c>
+      <c r="D45">
+        <v>220</v>
       </c>
       <c r="E45" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F45">
         <v>1</v>
       </c>
       <c r="G45">
-        <v>3.1E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H45">
         <f t="shared" si="0"/>
-        <v>3.1E-2</v>
+        <v>0.09</v>
       </c>
       <c r="I45" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C46" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="D46" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E46" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F46">
         <v>1</v>
       </c>
       <c r="G46">
-        <v>1.9E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="H46">
         <f t="shared" si="0"/>
-        <v>1.9E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="I46" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>170</v>
+        <v>57</v>
       </c>
       <c r="C47" t="s">
         <v>28</v>
@@ -2570,10 +2539,10 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C48" t="s">
         <v>28</v>
@@ -2600,10 +2569,10 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C49" t="s">
         <v>28</v>
@@ -2630,70 +2599,70 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>61</v>
+        <v>171</v>
       </c>
       <c r="C50" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D50" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E50" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F50">
         <v>1</v>
       </c>
       <c r="G50">
-        <v>1.2E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="H50">
         <f t="shared" si="0"/>
-        <v>1.2E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="I50" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>173</v>
+        <v>61</v>
       </c>
       <c r="C51" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="D51" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="E51" t="s">
-        <v>174</v>
+        <v>63</v>
       </c>
       <c r="F51">
         <v>1</v>
       </c>
       <c r="G51">
-        <v>0.1</v>
+        <v>1.2E-2</v>
       </c>
       <c r="H51">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>1.2E-2</v>
       </c>
       <c r="I51" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C52" t="s">
         <v>28</v>
@@ -2702,7 +2671,7 @@
         <v>16</v>
       </c>
       <c r="E52" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F52">
         <v>1</v>
@@ -2720,10 +2689,10 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>229</v>
+        <v>174</v>
       </c>
       <c r="C53" t="s">
         <v>28</v>
@@ -2732,7 +2701,7 @@
         <v>16</v>
       </c>
       <c r="E53" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -2750,10 +2719,10 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>176</v>
+        <v>228</v>
       </c>
       <c r="C54" t="s">
         <v>28</v>
@@ -2762,7 +2731,7 @@
         <v>16</v>
       </c>
       <c r="E54" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F54">
         <v>1</v>
@@ -2780,43 +2749,43 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>66</v>
+        <v>175</v>
       </c>
       <c r="C55" t="s">
-        <v>177</v>
+        <v>28</v>
       </c>
       <c r="D55" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="E55" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="F55">
         <v>1</v>
       </c>
       <c r="G55">
-        <v>1.2E-2</v>
+        <v>0.1</v>
       </c>
       <c r="H55">
         <f t="shared" si="0"/>
-        <v>1.2E-2</v>
+        <v>0.1</v>
       </c>
       <c r="I55" t="s">
-        <v>178</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>181</v>
+        <v>66</v>
       </c>
       <c r="C56" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D56" t="s">
         <v>65</v>
@@ -2835,18 +2804,18 @@
         <v>1.2E-2</v>
       </c>
       <c r="I56" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C57" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D57" t="s">
         <v>65</v>
@@ -2865,18 +2834,18 @@
         <v>1.2E-2</v>
       </c>
       <c r="I57" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C58" t="s">
-        <v>46</v>
+        <v>181</v>
       </c>
       <c r="D58" t="s">
         <v>65</v>
@@ -2895,15 +2864,15 @@
         <v>1.2E-2</v>
       </c>
       <c r="I58" t="s">
-        <v>68</v>
+        <v>182</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>148</v>
+        <v>184</v>
       </c>
       <c r="C59" t="s">
         <v>46</v>
@@ -2930,40 +2899,40 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>186</v>
+        <v>147</v>
       </c>
       <c r="C60" t="s">
         <v>46</v>
       </c>
       <c r="D60" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E60" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F60">
         <v>1</v>
       </c>
       <c r="G60">
-        <v>0.1</v>
+        <v>1.2E-2</v>
       </c>
       <c r="H60">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>1.2E-2</v>
       </c>
       <c r="I60" t="s">
-        <v>187</v>
+        <v>68</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="C61" t="s">
         <v>46</v>
@@ -2985,15 +2954,15 @@
         <v>0.1</v>
       </c>
       <c r="I61" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C62" t="s">
         <v>46</v>
@@ -3015,15 +2984,15 @@
         <v>0.1</v>
       </c>
       <c r="I62" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C63" t="s">
         <v>46</v>
@@ -3045,15 +3014,15 @@
         <v>0.1</v>
       </c>
       <c r="I63" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C64" t="s">
         <v>46</v>
@@ -3075,15 +3044,15 @@
         <v>0.1</v>
       </c>
       <c r="I64" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C65" t="s">
         <v>46</v>
@@ -3105,15 +3074,15 @@
         <v>0.1</v>
       </c>
       <c r="I65" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>145</v>
+        <v>188</v>
       </c>
       <c r="C66" t="s">
         <v>46</v>
@@ -3135,15 +3104,15 @@
         <v>0.1</v>
       </c>
       <c r="I66" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>204</v>
+        <v>144</v>
       </c>
       <c r="C67" t="s">
         <v>46</v>
@@ -3161,19 +3130,19 @@
         <v>0.1</v>
       </c>
       <c r="H67">
-        <f t="shared" ref="H67:H116" si="1">G67*F67</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="I67" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C68" t="s">
         <v>46</v>
@@ -3191,19 +3160,19 @@
         <v>0.1</v>
       </c>
       <c r="H68">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H68:H117" si="1">G68*F68</f>
         <v>0.1</v>
       </c>
       <c r="I68" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C69" t="s">
         <v>46</v>
@@ -3225,15 +3194,15 @@
         <v>0.1</v>
       </c>
       <c r="I69" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C70" t="s">
         <v>46</v>
@@ -3255,15 +3224,15 @@
         <v>0.1</v>
       </c>
       <c r="I70" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C71" t="s">
         <v>46</v>
@@ -3285,15 +3254,15 @@
         <v>0.1</v>
       </c>
       <c r="I71" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C72" t="s">
         <v>46</v>
@@ -3315,15 +3284,15 @@
         <v>0.1</v>
       </c>
       <c r="I72" t="s">
-        <v>64</v>
+        <v>202</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>237</v>
+        <v>208</v>
       </c>
       <c r="C73" t="s">
         <v>46</v>
@@ -3350,56 +3319,64 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>71</v>
+        <v>236</v>
       </c>
       <c r="C74" t="s">
-        <v>70</v>
+        <v>46</v>
+      </c>
+      <c r="D74" t="s">
+        <v>62</v>
+      </c>
+      <c r="E74" t="s">
+        <v>63</v>
       </c>
       <c r="F74">
         <v>1</v>
       </c>
       <c r="G74">
-        <v>18.64</v>
+        <v>0.1</v>
       </c>
       <c r="H74">
         <f t="shared" si="1"/>
-        <v>18.64</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>69</v>
+        <v>0.1</v>
+      </c>
+      <c r="I74" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>74</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3">
-        <v>1</v>
-      </c>
-      <c r="G75" s="3"/>
-      <c r="H75" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I75" s="4"/>
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
+        <v>71</v>
+      </c>
+      <c r="C75" t="s">
+        <v>70</v>
+      </c>
+      <c r="F75">
+        <v>1</v>
+      </c>
+      <c r="G75">
+        <v>18.64</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="1"/>
+        <v>18.64</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>72</v>
@@ -3418,10 +3395,10 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>72</v>
@@ -3436,44 +3413,36 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I77" s="3"/>
+      <c r="I77" s="4"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>77</v>
-      </c>
-      <c r="B78" t="s">
-        <v>213</v>
-      </c>
-      <c r="C78" t="s">
-        <v>28</v>
-      </c>
-      <c r="D78">
+        <v>76</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3">
+        <v>1</v>
+      </c>
+      <c r="G78" s="3"/>
+      <c r="H78" s="3">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E78" t="s">
-        <v>29</v>
-      </c>
-      <c r="F78">
-        <v>1</v>
-      </c>
-      <c r="G78">
-        <v>0.1</v>
-      </c>
-      <c r="H78">
-        <f t="shared" si="1"/>
-        <v>0.1</v>
-      </c>
-      <c r="I78" t="s">
-        <v>30</v>
-      </c>
+      <c r="I78" s="3"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>246</v>
+        <v>212</v>
       </c>
       <c r="C79" t="s">
         <v>28</v>
@@ -3500,10 +3469,10 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C80" t="s">
         <v>28</v>
@@ -3530,10 +3499,10 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C81" t="s">
         <v>28</v>
@@ -3560,10 +3529,10 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C82" t="s">
         <v>28</v>
@@ -3590,10 +3559,10 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C83" t="s">
         <v>28</v>
@@ -3620,10 +3589,10 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C84" t="s">
         <v>28</v>
@@ -3650,10 +3619,10 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C85" t="s">
         <v>28</v>
@@ -3680,10 +3649,10 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C86" t="s">
         <v>28</v>
@@ -3710,10 +3679,10 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C87" t="s">
         <v>28</v>
@@ -3740,100 +3709,100 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>73</v>
+        <v>255</v>
       </c>
       <c r="C88" t="s">
-        <v>74</v>
-      </c>
-      <c r="D88" t="s">
-        <v>75</v>
+        <v>28</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
       </c>
       <c r="E88" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="F88">
         <v>1</v>
       </c>
       <c r="G88">
-        <v>1.08</v>
+        <v>0.1</v>
       </c>
       <c r="H88">
         <f t="shared" si="1"/>
-        <v>1.08</v>
+        <v>0.1</v>
       </c>
       <c r="I88" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C89" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D89" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E89" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F89">
         <v>1</v>
       </c>
       <c r="G89">
-        <v>2.1019999999999999</v>
+        <v>1.08</v>
       </c>
       <c r="H89">
         <f t="shared" si="1"/>
-        <v>2.1019999999999999</v>
+        <v>1.08</v>
       </c>
       <c r="I89" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>216</v>
+        <v>79</v>
       </c>
       <c r="C90" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D90" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E90" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="F90">
         <v>1</v>
       </c>
       <c r="G90">
-        <v>0.57999999999999996</v>
+        <v>2.1019999999999999</v>
       </c>
       <c r="H90">
         <f t="shared" si="1"/>
-        <v>0.57999999999999996</v>
+        <v>2.1019999999999999</v>
       </c>
       <c r="I90" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C91" t="s">
         <v>83</v>
@@ -3860,40 +3829,40 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C92" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="D92" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E92" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F92">
         <v>1</v>
       </c>
       <c r="G92">
-        <v>2.1000000000000001E-2</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="H92">
         <f t="shared" si="1"/>
-        <v>2.1000000000000001E-2</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="I92" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C93" t="s">
         <v>46</v>
@@ -3920,49 +3889,49 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C94" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
       <c r="D94" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E94" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F94">
         <v>1</v>
       </c>
       <c r="G94">
-        <v>8.4000000000000005E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="H94">
         <f t="shared" si="1"/>
-        <v>8.4000000000000005E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="I94" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C95" t="s">
         <v>90</v>
       </c>
       <c r="D95" t="s">
-        <v>91</v>
+        <v>257</v>
       </c>
       <c r="E95" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F95">
         <v>1</v>
@@ -3975,24 +3944,24 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="I95" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C96" t="s">
         <v>90</v>
       </c>
       <c r="D96" t="s">
-        <v>91</v>
+        <v>257</v>
       </c>
       <c r="E96" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F96">
         <v>1</v>
@@ -4005,31 +3974,34 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="I96" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>93</v>
+        <v>221</v>
       </c>
       <c r="C97" t="s">
-        <v>92</v>
+        <v>90</v>
+      </c>
+      <c r="D97" t="s">
+        <v>257</v>
       </c>
       <c r="E97" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F97">
         <v>1</v>
       </c>
       <c r="G97">
-        <v>9.23</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="H97">
         <f t="shared" si="1"/>
-        <v>9.23</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="I97" t="s">
         <v>94</v>
@@ -4037,70 +4009,67 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C98" t="s">
-        <v>100</v>
-      </c>
-      <c r="D98" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E98" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F98">
         <v>1</v>
       </c>
       <c r="G98">
-        <v>4.5999999999999999E-2</v>
+        <v>9.23</v>
       </c>
       <c r="H98">
         <f t="shared" si="1"/>
-        <v>4.5999999999999999E-2</v>
+        <v>9.23</v>
       </c>
       <c r="I98" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99">
+        <v>97</v>
+      </c>
+      <c r="B99" t="s">
         <v>98</v>
       </c>
-      <c r="B99" t="s">
-        <v>224</v>
-      </c>
       <c r="C99" t="s">
-        <v>28</v>
-      </c>
-      <c r="D99">
-        <v>475</v>
+        <v>99</v>
+      </c>
+      <c r="D99" t="s">
+        <v>97</v>
       </c>
       <c r="E99" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F99">
         <v>1</v>
       </c>
       <c r="G99">
-        <v>1.2999999999999999E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="H99">
         <f t="shared" si="1"/>
-        <v>1.2999999999999999E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="I99" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C100" t="s">
         <v>28</v>
@@ -4109,118 +4078,118 @@
         <v>475</v>
       </c>
       <c r="E100" t="s">
+        <v>102</v>
+      </c>
+      <c r="F100">
+        <v>1</v>
+      </c>
+      <c r="G100">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="H100">
+        <f t="shared" si="1"/>
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="I100" t="s">
         <v>103</v>
-      </c>
-      <c r="F100">
-        <v>1</v>
-      </c>
-      <c r="G100">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="H100">
-        <f t="shared" si="1"/>
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="I100" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C101" t="s">
-        <v>38</v>
-      </c>
-      <c r="D101" t="s">
-        <v>105</v>
+        <v>28</v>
+      </c>
+      <c r="D101">
+        <v>475</v>
       </c>
       <c r="E101" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F101">
         <v>1</v>
       </c>
       <c r="G101">
-        <v>2.3E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="H101">
         <f t="shared" si="1"/>
-        <v>2.3E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="I101" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C102" t="s">
-        <v>110</v>
+        <v>38</v>
       </c>
       <c r="D102" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E102" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F102">
         <v>1</v>
       </c>
       <c r="G102">
-        <v>2.8000000000000001E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="H102">
         <f t="shared" si="1"/>
-        <v>2.8000000000000001E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="I102" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>112</v>
+        <v>226</v>
       </c>
       <c r="C103" t="s">
-        <v>28</v>
-      </c>
-      <c r="D103">
-        <v>39</v>
+        <v>109</v>
+      </c>
+      <c r="D103" t="s">
+        <v>107</v>
       </c>
       <c r="E103" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F103">
         <v>1</v>
       </c>
       <c r="G103">
-        <v>1.2999999999999999E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="H103">
         <f t="shared" si="1"/>
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="I103" s="2" t="s">
-        <v>114</v>
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="I103" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>233</v>
+        <v>111</v>
       </c>
       <c r="C104" t="s">
         <v>28</v>
@@ -4229,28 +4198,28 @@
         <v>39</v>
       </c>
       <c r="E104" t="s">
+        <v>112</v>
+      </c>
+      <c r="F104">
+        <v>1</v>
+      </c>
+      <c r="G104">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="H104">
+        <f t="shared" si="1"/>
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="I104" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="F104">
-        <v>1</v>
-      </c>
-      <c r="G104">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="H104">
-        <f t="shared" si="1"/>
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="I104" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C105" t="s">
         <v>28</v>
@@ -4259,28 +4228,28 @@
         <v>39</v>
       </c>
       <c r="E105" t="s">
+        <v>112</v>
+      </c>
+      <c r="F105">
+        <v>1</v>
+      </c>
+      <c r="G105">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="H105">
+        <f t="shared" si="1"/>
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="I105" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="F105">
-        <v>1</v>
-      </c>
-      <c r="G105">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="H105">
-        <f t="shared" si="1"/>
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="I105" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C106" t="s">
         <v>28</v>
@@ -4289,88 +4258,91 @@
         <v>39</v>
       </c>
       <c r="E106" t="s">
+        <v>112</v>
+      </c>
+      <c r="F106">
+        <v>1</v>
+      </c>
+      <c r="G106">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="H106">
+        <f t="shared" si="1"/>
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="I106" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="F106">
-        <v>1</v>
-      </c>
-      <c r="G106">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="H106">
-        <f t="shared" si="1"/>
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="I106" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>115</v>
+        <v>238</v>
       </c>
       <c r="C107" t="s">
-        <v>116</v>
+        <v>28</v>
+      </c>
+      <c r="D107">
+        <v>39</v>
       </c>
       <c r="E107" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F107">
         <v>1</v>
       </c>
       <c r="G107">
-        <v>0.28999999999999998</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="H107">
         <f t="shared" si="1"/>
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="I107" t="s">
-        <v>118</v>
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="I107" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>235</v>
+        <v>114</v>
       </c>
       <c r="C108" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E108" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F108">
         <v>1</v>
       </c>
       <c r="G108">
-        <v>0.38400000000000001</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="H108">
         <f t="shared" si="1"/>
-        <v>0.38400000000000001</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="I108" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C109" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E109" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F109">
         <v>1</v>
@@ -4383,182 +4355,186 @@
         <v>0.38400000000000001</v>
       </c>
       <c r="I109" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>122</v>
+        <v>235</v>
       </c>
       <c r="C110" t="s">
-        <v>124</v>
-      </c>
-      <c r="D110" t="s">
-        <v>240</v>
+        <v>119</v>
       </c>
       <c r="E110" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F110">
         <v>1</v>
       </c>
       <c r="G110">
-        <v>1.6E-2</v>
+        <v>0.38400000000000001</v>
       </c>
       <c r="H110">
         <f t="shared" si="1"/>
-        <v>1.6E-2</v>
+        <v>0.38400000000000001</v>
       </c>
       <c r="I110" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C111" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D111" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E111" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F111">
         <v>1</v>
       </c>
       <c r="G111">
-        <v>1.2999999999999999E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="H111">
         <f t="shared" si="1"/>
-        <v>1.2999999999999999E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="I111" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C112" t="s">
-        <v>130</v>
+        <v>127</v>
+      </c>
+      <c r="D112" t="s">
+        <v>240</v>
       </c>
       <c r="E112" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="F112">
         <v>1</v>
       </c>
       <c r="G112">
-        <v>2.93</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="H112">
         <f t="shared" si="1"/>
-        <v>2.93</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="I112" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C113" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E113" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F113">
         <v>1</v>
       </c>
       <c r="G113">
-        <v>3.8</v>
+        <v>2.93</v>
       </c>
       <c r="H113">
         <f t="shared" si="1"/>
-        <v>3.8</v>
+        <v>2.93</v>
       </c>
       <c r="I113" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B114" t="s">
+        <v>131</v>
+      </c>
+      <c r="C114" t="s">
+        <v>134</v>
+      </c>
+      <c r="E114" t="s">
         <v>133</v>
       </c>
-      <c r="C114" t="s">
+      <c r="F114">
+        <v>1</v>
+      </c>
+      <c r="G114">
+        <v>3.8</v>
+      </c>
+      <c r="H114">
+        <f t="shared" si="1"/>
+        <v>3.8</v>
+      </c>
+      <c r="I114" t="s">
         <v>136</v>
-      </c>
-      <c r="E114" t="s">
-        <v>139</v>
-      </c>
-      <c r="F114">
-        <v>1</v>
-      </c>
-      <c r="G114">
-        <v>2.9</v>
-      </c>
-      <c r="H114">
-        <f t="shared" si="1"/>
-        <v>2.9</v>
-      </c>
-      <c r="I114" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>114</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="D115" s="3"/>
-      <c r="E115" s="3"/>
-      <c r="F115" s="3">
-        <v>1</v>
-      </c>
-      <c r="G115" s="3"/>
-      <c r="H115" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I115" s="3"/>
-      <c r="J115" s="3"/>
+        <v>113</v>
+      </c>
+      <c r="B115" t="s">
+        <v>132</v>
+      </c>
+      <c r="C115" t="s">
+        <v>135</v>
+      </c>
+      <c r="E115" t="s">
+        <v>138</v>
+      </c>
+      <c r="F115">
+        <v>1</v>
+      </c>
+      <c r="G115">
+        <v>2.9</v>
+      </c>
+      <c r="H115">
+        <f t="shared" si="1"/>
+        <v>2.9</v>
+      </c>
+      <c r="I115" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B116" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C116" s="3" t="s">
         <v>244</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>245</v>
       </c>
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
@@ -4574,18 +4550,41 @@
       <c r="J116" s="3"/>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H117">
-        <f>SUM(H2:H116)</f>
+      <c r="A117">
+        <v>115</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D117" s="3"/>
+      <c r="E117" s="3"/>
+      <c r="F117" s="3">
+        <v>1</v>
+      </c>
+      <c r="G117" s="3"/>
+      <c r="H117" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I117" s="3"/>
+      <c r="J117" s="3"/>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H118">
+        <f>SUM(H2:H117)</f>
         <v>61.157000000000011</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I106" r:id="rId1"/>
-    <hyperlink ref="I74" r:id="rId2"/>
-    <hyperlink ref="I103" r:id="rId3"/>
-    <hyperlink ref="I105" r:id="rId4"/>
-    <hyperlink ref="I104" r:id="rId5"/>
+    <hyperlink ref="I107" r:id="rId1"/>
+    <hyperlink ref="I75" r:id="rId2"/>
+    <hyperlink ref="I104" r:id="rId3"/>
+    <hyperlink ref="I106" r:id="rId4"/>
+    <hyperlink ref="I105" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>